<commit_message>
working on the crosswalk isco 68 to 88.Version 1.0
</commit_message>
<xml_diff>
--- a/MONO131/CANJEM_IPUMS analysis/intermediate data/isco68to88V1.xlsx
+++ b/MONO131/CANJEM_IPUMS analysis/intermediate data/isco68to88V1.xlsx
@@ -410,7 +410,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Both missing</t>
+          <t>IPUMS Military</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -9125,12 +9130,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G257" t="inlineStr">
-        <is>
-          <t>310</t>
+          <t>Low resolution</t>
         </is>
       </c>
     </row>
@@ -11350,12 +11350,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G323" t="inlineStr">
-        <is>
-          <t>410</t>
+          <t>Low resolution</t>
         </is>
       </c>
     </row>
@@ -11520,12 +11515,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G328" t="inlineStr">
-        <is>
-          <t>410</t>
+          <t>Low resolution</t>
         </is>
       </c>
     </row>
@@ -33125,12 +33115,7 @@
       </c>
       <c r="F969" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G969" t="inlineStr">
-        <is>
-          <t>840</t>
+          <t>Low resolution</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
crosswalk update : exclussion of supervisors (no ISCO88 code for them)
</commit_message>
<xml_diff>
--- a/MONO131/CANJEM_IPUMS analysis/intermediate data/isco68to88V1.xlsx
+++ b/MONO131/CANJEM_IPUMS analysis/intermediate data/isco68to88V1.xlsx
@@ -16650,12 +16650,7 @@
       </c>
       <c r="F480" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G480" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16680,12 +16675,7 @@
       </c>
       <c r="F481" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G481" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16710,12 +16700,7 @@
       </c>
       <c r="F482" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G482" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16740,12 +16725,7 @@
       </c>
       <c r="F483" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G483" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16770,12 +16750,7 @@
       </c>
       <c r="F484" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G484" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16800,12 +16775,7 @@
       </c>
       <c r="F485" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G485" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16830,12 +16800,7 @@
       </c>
       <c r="F486" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G486" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16860,12 +16825,7 @@
       </c>
       <c r="F487" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G487" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16890,12 +16850,7 @@
       </c>
       <c r="F488" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G488" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16920,12 +16875,7 @@
       </c>
       <c r="F489" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G489" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16950,12 +16900,7 @@
       </c>
       <c r="F490" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G490" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>
@@ -16980,12 +16925,7 @@
       </c>
       <c r="F491" t="inlineStr">
         <is>
-          <t>CAPS missing</t>
-        </is>
-      </c>
-      <c r="G491" t="inlineStr">
-        <is>
-          <t>751</t>
+          <t>supervisors</t>
         </is>
       </c>
     </row>

</xml_diff>